<commit_message>
updates and tweaks to bib display
</commit_message>
<xml_diff>
--- a/data/schedule-condensed.xlsx
+++ b/data/schedule-condensed.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/vsd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE788A6-6744-7249-9CC1-9F6CC81C04E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93A0B28-F4F7-114B-A0FD-1B4FA6EFBDEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="54">
   <si>
     <t>group</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>/content/02-content</t>
+  </si>
+  <si>
+    <t>/content/03-content</t>
   </si>
 </sst>
 </file>
@@ -677,6 +680,9 @@
       <c r="F4" t="s">
         <v>13</v>
       </c>
+      <c r="H4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
wk03 stuff; wk04 readings
</commit_message>
<xml_diff>
--- a/data/schedule-condensed.xlsx
+++ b/data/schedule-condensed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kjhealy/Documents/courses/vsd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E815E4EE-AB89-F44F-89F1-4D0C2F582DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{841E5F2F-B0CA-D64F-85AE-929A79560B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1380" yWindow="1540" windowWidth="26840" windowHeight="15940" xr2:uid="{FF444104-2C96-9340-A7A7-D0D5BB267F7C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="55">
   <si>
     <t>group</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>/assignment/03-problem-set</t>
+  </si>
+  <si>
+    <t>/content/04-content</t>
   </si>
 </sst>
 </file>
@@ -572,7 +575,7 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,6 +722,9 @@
       <c r="F5" t="s">
         <v>36</v>
       </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">

</xml_diff>